<commit_message>
added duplicate insertion prevention
</commit_message>
<xml_diff>
--- a/excel-uploader-backend/mysheet.xlsx
+++ b/excel-uploader-backend/mysheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumit\Documents\node js\excel-uploader\excel-uploader-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA00483-0F36-48E9-BB11-C124A2F86AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023A42B8-CB27-4BAE-9247-56B8B1D9A663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{6A2DFE61-DFBF-4966-B582-368081D132DF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>ced19i057@iiitdm.ac.in</t>
+  </si>
+  <si>
+    <t>ced19i001@iiitdm.ac.in</t>
+  </si>
+  <si>
+    <t>ced19i034@iiitdm.ac.in</t>
+  </si>
+  <si>
+    <t>some</t>
+  </si>
+  <si>
+    <t>ced19i098@iiitdm.ac.in</t>
   </si>
 </sst>
 </file>
@@ -558,10 +570,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02ED9E16-76EF-44F7-B975-5EAF5149B362}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -570,7 +582,7 @@
     <col min="3" max="3" width="19.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -580,8 +592,11 @@
       <c r="C1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -591,8 +606,11 @@
       <c r="C2">
         <v>6456766543</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -602,8 +620,11 @@
       <c r="C3">
         <v>12121212121</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -613,8 +634,11 @@
       <c r="C4">
         <v>2123232444</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -624,8 +648,11 @@
       <c r="C5">
         <v>64567662321</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -634,6 +661,51 @@
       </c>
       <c r="C6">
         <v>876789878</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>876789878</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>2123232444</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>2123232444</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -643,6 +715,9 @@
     <hyperlink ref="A4" r:id="rId3" xr:uid="{9A4EB12B-60AE-40BD-92DB-28A1CE9A3F1C}"/>
     <hyperlink ref="A5" r:id="rId4" xr:uid="{B18D60E4-2E4A-415D-9B49-962DFA5E61CE}"/>
     <hyperlink ref="A6" r:id="rId5" xr:uid="{2A5E133D-60FB-43FF-B751-35C75B731311}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{33F47BFD-05BA-4736-A711-8CF4726BFCB1}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{032A0682-A391-4D62-9F8A-9E195D134D72}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{FE63325D-B1C1-4A6C-9D7D-DD6B1A790A22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>